<commit_message>
Test plan team member report updated
Test plan team member report updated
</commit_message>
<xml_diff>
--- a/docs/deliverable3/Getana_Deliverable_3_TeamMemberReport_5.xlsx
+++ b/docs/deliverable3/Getana_Deliverable_3_TeamMemberReport_5.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Arpit" sheetId="1" r:id="rId1"/>
@@ -106,7 +106,7 @@
     <t>Out sick during Usability Study</t>
   </si>
   <si>
-    <t xml:space="preserve">Release new version APK for deliverable 3; Updated URN and SRS documents; Participated in Usability Study, created script, recorded and took note of activities; Updated Kanban board. </t>
+    <t xml:space="preserve">Release new version APK for deliverable 3; Updated URN and SRS documents; Organized Usability Study, created script, recorded and took note of activities; Updated Kanban board. </t>
   </si>
 </sst>
 </file>
@@ -857,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="B11" sqref="B10:B11"/>
+    <sheetView zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -944,7 +944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK10"/>
   <sheetViews>
-    <sheetView zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Team member report push
</commit_message>
<xml_diff>
--- a/docs/deliverable3/Getana_Deliverable_3_TeamMemberReport_5.xlsx
+++ b/docs/deliverable3/Getana_Deliverable_3_TeamMemberReport_5.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wuyon\Documents\GitHub\RaiderNAV\docs\deliverable3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brodywilliams/Repositories/RaiderNAV/docs/deliverable3/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E75670-28EA-1B4F-A6D6-C7D485B54CDF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="989" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arpit" sheetId="1" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="32">
   <si>
     <t>Team Member Report – Sprint 5</t>
   </si>
@@ -55,9 +56,6 @@
     <t>Role duties and work to be performed next week(sprint):</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>Issues encountered:</t>
   </si>
   <si>
@@ -106,25 +104,34 @@
     <t xml:space="preserve">Security requirment should be FR, it's too late to get aknowledged </t>
   </si>
   <si>
-    <t>Unit test</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
     <t>Get familiar with Github</t>
   </si>
   <si>
-    <t>Release new version APK for deliverable 3; Updated URN and SRS documents; Participated in Usability Study, created script, recorded and took note of activities; Updated Kanban board. Etc</t>
-  </si>
-  <si>
-    <t>Updated product backlog; Updated SRS, URN documents; Participated in Usability Study, created forms for it; Create software architecture and design pattern document; etc</t>
+    <t>Scrum Master</t>
+  </si>
+  <si>
+    <t>Product Owner</t>
+  </si>
+  <si>
+    <t>Unfamiliarity with Unit Testing</t>
+  </si>
+  <si>
+    <t>Out of Town 4/11-4/16</t>
+  </si>
+  <si>
+    <t>Updated product backlog; Updated SRS, URN documents; Participated in Usability Study, created forms for it; Create software architecture and design pattern document; Updated SRS document; Added Use case 34; PDFized several documents</t>
+  </si>
+  <si>
+    <t>Release new version APK for deliverable 3; Updated URN and SRS documents; Participated in Usability Study, created script, recorded and took note of activities; Updated Kanban board.; Created misuse case diagram for use case 34; Reworded privacy notification; Completed acceptance &amp; unit testing; Combined elements into test plan document</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -203,7 +210,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -515,41 +522,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK10"/>
   <sheetViews>
     <sheetView zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="71.42578125" style="1"/>
-    <col min="2" max="2" width="33.7109375" style="1"/>
-    <col min="3" max="1025" width="11.140625" style="1"/>
+    <col min="1" max="1" width="71.5" style="1"/>
+    <col min="2" max="2" width="33.6640625" style="1"/>
+    <col min="3" max="1025" width="11.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2"/>
       <c r="B2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4"/>
       <c r="B4"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -557,7 +564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -565,41 +572,41 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:2" ht="36" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -608,86 +615,86 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK10"/>
   <sheetViews>
     <sheetView zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="71.42578125" style="1"/>
-    <col min="2" max="2" width="38.42578125" style="1"/>
-    <col min="3" max="1025" width="11.140625" style="1"/>
+    <col min="1" max="1" width="71.5" style="1"/>
+    <col min="2" max="2" width="38.5" style="1"/>
+    <col min="3" max="1025" width="11.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2"/>
       <c r="B2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4"/>
       <c r="B4"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="126" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="144" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -701,49 +708,49 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK10"/>
   <sheetViews>
     <sheetView zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="71.42578125" style="1"/>
-    <col min="2" max="2" width="34.7109375" style="1"/>
-    <col min="3" max="1025" width="11.140625" style="1"/>
+    <col min="1" max="1" width="71.5" style="1"/>
+    <col min="2" max="2" width="34.6640625" style="1"/>
+    <col min="3" max="1025" width="11.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2"/>
       <c r="B2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4"/>
       <c r="B4"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -751,36 +758,36 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:2" ht="90" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -794,49 +801,49 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMK10"/>
   <sheetViews>
     <sheetView zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="71.42578125" style="1"/>
-    <col min="2" max="2" width="38.5703125" style="1"/>
-    <col min="3" max="1025" width="11.140625" style="1"/>
+    <col min="1" max="1" width="71.5" style="1"/>
+    <col min="2" max="2" width="38.5" style="1"/>
+    <col min="3" max="1025" width="11.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2"/>
       <c r="B2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4"/>
       <c r="B4"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -844,33 +851,36 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:2" ht="90" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
+      <c r="B10" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -884,49 +894,49 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMK10"/>
   <sheetViews>
-    <sheetView zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="71.42578125" style="1"/>
-    <col min="2" max="2" width="40.85546875" style="1"/>
-    <col min="3" max="1025" width="11.140625" style="1"/>
+    <col min="1" max="1" width="71.5" style="1"/>
+    <col min="2" max="2" width="40.83203125" style="1"/>
+    <col min="3" max="1025" width="11.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2"/>
       <c r="B2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4"/>
       <c r="B4"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -934,36 +944,36 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="126" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:2" ht="198" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -977,86 +987,86 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AMK10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="87.5703125" style="1"/>
-    <col min="2" max="2" width="44.140625" style="1"/>
-    <col min="3" max="1025" width="11.140625" style="1"/>
+    <col min="1" max="1" width="87.5" style="1"/>
+    <col min="2" max="2" width="44.1640625" style="1"/>
+    <col min="3" max="1025" width="11.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2"/>
       <c r="B2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4"/>
       <c r="B4"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="162" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="144" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>